<commit_message>
Fixed ro-crate-metadata file extension  and rebuilt
</commit_message>
<xml_diff>
--- a/sample-crate/ro-crate-metadata.xlsx
+++ b/sample-crate/ro-crate-metadata.xlsx
@@ -1,35 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13942B10-BB02-F842-BFFC-9499EAE9F9A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="RootDataset" sheetId="1" r:id="rId1"/>
-    <sheet name="@context" sheetId="2" r:id="rId2"/>
-    <sheet name="@type=Dataset" sheetId="3" r:id="rId3"/>
-    <sheet name="@type=File" sheetId="4" r:id="rId4"/>
-    <sheet name="@type=Person" sheetId="5" r:id="rId5"/>
-    <sheet name="@type=Organization" sheetId="6" r:id="rId6"/>
-    <sheet name="@type=Place" sheetId="7" r:id="rId7"/>
-    <sheet name="@type=ScholarlyArticle" sheetId="8" r:id="rId8"/>
-    <sheet name="@type=IndividualProduct" sheetId="9" r:id="rId9"/>
-    <sheet name="@type=CreateAction" sheetId="10" r:id="rId10"/>
-    <sheet name="@type=DataDownload" sheetId="11" r:id="rId11"/>
-    <sheet name="@type=CreativeWork" sheetId="12" r:id="rId12"/>
-    <sheet name="@type=SoftwareApplication" sheetId="13" r:id="rId13"/>
-    <sheet name="@type=ContactPoint" sheetId="14" r:id="rId14"/>
-    <sheet name="@type=website" sheetId="15" r:id="rId15"/>
+    <sheet sheetId="1" name="RootDataset" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="@context" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="@type=Dataset" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="@type=File" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="@type=Person" state="visible" r:id="rId8"/>
+    <sheet sheetId="6" name="@type=Organization" state="visible" r:id="rId9"/>
+    <sheet sheetId="7" name="@type=Place" state="visible" r:id="rId10"/>
+    <sheet sheetId="8" name="@type=ScholarlyArticle" state="visible" r:id="rId11"/>
+    <sheet sheetId="9" name="@type=IndividualProduct" state="visible" r:id="rId12"/>
+    <sheet sheetId="10" name="@type=CreateAction" state="visible" r:id="rId13"/>
+    <sheet sheetId="11" name="@type=DataDownload" state="visible" r:id="rId14"/>
+    <sheet sheetId="12" name="@type=CreativeWork" state="visible" r:id="rId15"/>
+    <sheet sheetId="13" name="@type=SoftwareApplication" state="visible" r:id="rId16"/>
+    <sheet sheetId="14" name="@type=website" state="visible" r:id="rId17"/>
+    <sheet sheetId="15" name="@type=ContactPoint" state="visible" r:id="rId18"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="178">
   <si>
     <t>Name</t>
   </si>
@@ -118,6 +114,9 @@
     <t>name</t>
   </si>
   <si>
+    <t>Sample dataset for RO-Crate v1.1</t>
+  </si>
+  <si>
     <t>publisher</t>
   </si>
   <si>
@@ -127,6 +126,9 @@
     <t>temporalCoverage</t>
   </si>
   <si>
+    <t>2017</t>
+  </si>
+  <si>
     <t>lots_of_little_files/</t>
   </si>
   <si>
@@ -145,7 +147,7 @@
     <t>Pictures</t>
   </si>
   <si>
-    <t>["pics/2017-06-11 12.56.14.jpg", "pics/sepia_fence.jpg", "pics/thumbs/"]</t>
+    <t/>
   </si>
   <si>
     <t>pics/thumbs/</t>
@@ -163,6 +165,9 @@
     <t>creator</t>
   </si>
   <si>
+    <t>dateModified</t>
+  </si>
+  <si>
     <t>encodingFormat</t>
   </si>
   <si>
@@ -172,7 +177,34 @@
     <t>thumbnail</t>
   </si>
   <si>
-    <t>dateModified</t>
+    <t>LICENSE</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>35149</t>
+  </si>
+  <si>
+    <t>2021-01-19T15:47:13+11:00</t>
+  </si>
+  <si>
+    <t>["https://www.nationalarchives.gov.uk/PRONOM/pronom", text/plain]</t>
+  </si>
+  <si>
+    <t>README.md</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>index.html</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>"https://www.nationalarchives.gov.uk/PRONOM/pronom"</t>
   </si>
   <si>
     <t>pics/2017-06-11 12.56.14.jpg</t>
@@ -217,9 +249,6 @@
     <t>pics/thumbs/2017-06-11 12.56.14.png</t>
   </si>
   <si>
-    <t>File</t>
-  </si>
-  <si>
     <t>20594</t>
   </si>
   <si>
@@ -235,27 +264,6 @@
     <t>20524</t>
   </si>
   <si>
-    <t>LICENSE</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>["https://www.nationalarchives.gov.uk/PRONOM/pronom", text/plain]</t>
-  </si>
-  <si>
-    <t>2021-01-19T15:47:13+11:00</t>
-  </si>
-  <si>
-    <t>README.md</t>
-  </si>
-  <si>
-    <t>index.html</t>
-  </si>
-  <si>
-    <t>["https://www.nationalarchives.gov.uk/PRONOM/pronom"]</t>
-  </si>
-  <si>
     <t>affiliation</t>
   </si>
   <si>
@@ -484,9 +492,6 @@
     <t>path</t>
   </si>
   <si>
-    <t>contentUrl</t>
-  </si>
-  <si>
     <t>#picsdistro</t>
   </si>
   <si>
@@ -499,6 +504,9 @@
     <t>https://data.research.uts.edu.au/examples/ro-crate/examples/src/downloads/sample.zip</t>
   </si>
   <si>
+    <t>[https://data.research.uts.edu.au/examples/ro-crate/examples/src/downloads/sample.zip, ]</t>
+  </si>
+  <si>
     <t>zip</t>
   </si>
   <si>
@@ -526,7 +534,16 @@
     <t>ImageMagick</t>
   </si>
   <si>
-    <t> ImageMagick 7.0.8-2 Q16 x86_64 2018-06-19</t>
+    <t xml:space="preserve"> ImageMagick 7.0.8-2 Q16 x86_64 2018-06-19</t>
+  </si>
+  <si>
+    <t>https://www.nationalarchives.gov.uk/PRONOM/pronom</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>Plain Text File</t>
   </si>
   <si>
     <t>contactType</t>
@@ -542,31 +559,19 @@
   </si>
   <si>
     <t>Contact Peter Sefton</t>
-  </si>
-  <si>
-    <t>https://www.nationalarchives.gov.uk/PRONOM/pronom</t>
-  </si>
-  <si>
-    <t>website</t>
-  </si>
-  <si>
-    <t>Plain Text File</t>
-  </si>
-  <si>
-    <t>Sample dataset for RO-Crate v1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -929,21 +934,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B17" sqref="B17"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -951,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -959,7 +964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -967,7 +972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -975,7 +980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -983,7 +988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -991,7 +996,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -999,7 +1004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1007,7 +1012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1015,7 +1020,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1023,7 +1028,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1031,7 +1036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1039,7 +1044,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1047,7 +1052,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1055,48 +1060,45 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17">
-        <v>2017</v>
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="9" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1104,103 +1106,100 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G1" t="s">
         <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="I1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" t="s">
         <v>147</v>
       </c>
-      <c r="G3" t="s">
-        <v>148</v>
-      </c>
-      <c r="H3" t="s">
-        <v>143</v>
-      </c>
       <c r="I3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="6" width="20" customWidth="1"/>
+    <col min="1" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1208,67 +1207,61 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D1" t="s">
         <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>156</v>
+      </c>
+      <c r="C3" t="s">
+        <v>159</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1282,38 +1275,35 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1321,50 +1311,83 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
         <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1372,90 +1395,48 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E2" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="3" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1465,24 +1446,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1499,74 +1475,69 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="20" customWidth="1"/>
+    <col min="1" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1574,212 +1545,263 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
       <c r="J1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
       </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
       <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>57</v>
       </c>
-      <c r="F3" t="s">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
         <v>58</v>
       </c>
-      <c r="G3" t="s">
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
         <v>59</v>
       </c>
-      <c r="H3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>61</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>62</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
         <v>63</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G5" t="s">
         <v>64</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H5" t="s">
         <v>65</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" t="s">
         <v>67</v>
       </c>
-      <c r="F5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6">
-        <v>35149</v>
-      </c>
-      <c r="E6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" t="s">
-        <v>68</v>
-      </c>
       <c r="J6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7">
-        <v>31</v>
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>75</v>
       </c>
       <c r="H7" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8">
-        <v>17</v>
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
-      </c>
-      <c r="J8" t="s">
-        <v>71</v>
+        <v>76</v>
+      </c>
+      <c r="I8" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1787,68 +1809,65 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1865,91 +1884,92 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
         <v>92</v>
       </c>
-      <c r="D3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" t="s">
-        <v>88</v>
-      </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1957,62 +1977,59 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2029,41 +2046,38 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2071,78 +2085,78 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="G1" t="s">
         <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
         <v>122</v>
       </c>
-      <c r="G2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" t="s">
-        <v>118</v>
-      </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="H3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed file handling in rocxl
</commit_message>
<xml_diff>
--- a/sample-crate/ro-crate-metadata.xlsx
+++ b/sample-crate/ro-crate-metadata.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="170">
   <si>
     <t>Name</t>
   </si>
@@ -135,6 +135,9 @@
     <t>This directory contains many small files, that we’re not going to describe in detail.</t>
   </si>
   <si>
+    <t>[]</t>
+  </si>
+  <si>
     <t>Too many files</t>
   </si>
   <si>
@@ -144,21 +147,24 @@
     <t>This directory contains the images for the research project</t>
   </si>
   <si>
+    <t>["pics/2017-06-11 12.56.14.jpg", "pics/sepia_fence.jpg", "pics/thumbs/"]</t>
+  </si>
+  <si>
     <t>Pictures</t>
   </si>
   <si>
+    <t>pics/thumbs/</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>pics/thumbs/</t>
+    <t>["pics/thumbs/2017-06-11 12.56.14.png", "pics/thumbs/sepia_fence.png"]</t>
   </si>
   <si>
     <t>Thumbnails</t>
   </si>
   <si>
-    <t>["pics/thumbs/2017-06-11 12.56.14.png", "pics/thumbs/sepia_fence.png"]</t>
-  </si>
-  <si>
     <t>contentSize</t>
   </si>
   <si>
@@ -177,370 +183,340 @@
     <t>thumbnail</t>
   </si>
   <si>
-    <t>LICENSE</t>
+    <t>pics/2017-06-11 12.56.14.jpg</t>
+  </si>
+  <si>
+    <t>[File, ImageObject]</t>
+  </si>
+  <si>
+    <t>2021-04-21T11:27:03+10:00</t>
+  </si>
+  <si>
+    <t>Depicts a fence at a disused motor racing venue with the front part of a slightly out of focus black dog in the foreground.</t>
+  </si>
+  <si>
+    <t>["https://www.nationalarchives.gov.uk/PRONOM/fmt/645", image/jpeg]</t>
+  </si>
+  <si>
+    <t>http://www.nationalarchives.gov.uk/PRONOM/fmt/645</t>
+  </si>
+  <si>
+    <t>"pics/thumbs/2017-06-11 12.56.14.png"</t>
+  </si>
+  <si>
+    <t>pics/sepia_fence.jpg</t>
+  </si>
+  <si>
+    <t>Sepia tone version of my fence/dog pic</t>
+  </si>
+  <si>
+    <t>["https://www.nationalarchives.gov.uk/PRONOM/fmt/43", image/jpeg]</t>
+  </si>
+  <si>
+    <t>http://www.nationalarchives.gov.uk/PRONOM/fmt/43</t>
+  </si>
+  <si>
+    <t>"pics/thumbs/sepia_fence.png"</t>
+  </si>
+  <si>
+    <t>pics/thumbs/2017-06-11 12.56.14.png</t>
   </si>
   <si>
     <t>File</t>
   </si>
   <si>
-    <t>35149</t>
-  </si>
-  <si>
-    <t>2021-01-19T15:47:13+11:00</t>
-  </si>
-  <si>
-    <t>["https://www.nationalarchives.gov.uk/PRONOM/pronom", text/plain]</t>
-  </si>
-  <si>
-    <t>README.md</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>index.html</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>"https://www.nationalarchives.gov.uk/PRONOM/pronom"</t>
-  </si>
-  <si>
-    <t>pics/2017-06-11 12.56.14.jpg</t>
-  </si>
-  <si>
-    <t>[File, ImageObject]</t>
-  </si>
-  <si>
-    <t>5114778</t>
-  </si>
-  <si>
-    <t>Depicts a fence at a disused motor racing venue with the front part of a slightly out of focus black dog in the foreground.</t>
+    <t>["https://www.nationalarchives.gov.uk/PRONOM/fmt/11", image/png]</t>
+  </si>
+  <si>
+    <t>http://www.nationalarchives.gov.uk/PRONOM/fmt/11</t>
+  </si>
+  <si>
+    <t>pics/thumbs/sepia_fence.png</t>
+  </si>
+  <si>
+    <t>affiliation</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>familyName</t>
+  </si>
+  <si>
+    <t>givenName</t>
+  </si>
+  <si>
+    <t>http://orcid.org/0000-0002-3545-944X</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>mailto:peter.sefton@uts.edu.au</t>
+  </si>
+  <si>
+    <t>pt@ptsefton.com</t>
+  </si>
+  <si>
+    <t>Sefton</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Peter Sefton</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>http://ands.org.au</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>The core purpose of the Australian National Data Service (ANDS) is to make Australia’s research data assets more valuable for researchers, research institutions and the nation.</t>
+  </si>
+  <si>
+    <t>Australian National Data Service</t>
+  </si>
+  <si>
+    <t>http://eresearch.uts.edu.au/projects/provisioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The University of Technology Sydney Provisioner project is </t>
+  </si>
+  <si>
+    <t>Provisioner Project</t>
+  </si>
+  <si>
+    <t>["https://ror.org/0384j8v12", "http://ands.org.au"]</t>
+  </si>
+  <si>
+    <t>https://github.com/UTS-eResearch/projects/datacrate</t>
+  </si>
+  <si>
+    <t>The DataCrate project is to write the spec for DataCrate, of which this is an example. The DataCrate project is part of the University of Technology Sydney's Provisioner project, which was part-funded by the Australian National Data Service (ANDS) - now part of the Australian Research Data Commons (ARDC).</t>
+  </si>
+  <si>
+    <t>DataCrate Project</t>
+  </si>
+  <si>
+    <t>https://ror.org/0384j8v12</t>
+  </si>
+  <si>
+    <t>University of Technology Sydney</t>
+  </si>
+  <si>
+    <t>Broadway, 2007, NSW Australia</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>geo</t>
+  </si>
+  <si>
+    <t>http://www.geonames.org/8152662/catalina-park.html</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Catalina_Park</t>
+  </si>
+  <si>
+    <t>Katoomba, NSW</t>
+  </si>
+  <si>
+    <t>Catalina Park is a disused motor racing venue, located at Katoomba, in the Blue Mountains, New South Wales, Australia, and is recognised as an Aboriginal Place due to the long association of the local Gundungarra and Darug clans to the area.</t>
+  </si>
+  <si>
+    <t>{"@id":"#3e53e101-db05-49ad-a988-d97e484c2310","@type":"GeoCoordinates","latitude":"-33.7152","longitude":"150.30119","name":"Latitude: -33.7152, Longitude: 150.30119"}</t>
+  </si>
+  <si>
+    <t>Catalina Park</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1000/123456</t>
+  </si>
+  <si>
+    <t>ScholarlyArticle</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>This is an example publication with a dodgy DOI</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>serialNumber</t>
+  </si>
+  <si>
+    <t>#EPL1</t>
+  </si>
+  <si>
+    <t>IndividualProduct</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Olympus_PEN_E-PL1</t>
+  </si>
+  <si>
+    <t>Olympus camera with Panasonic 20mm lens</t>
+  </si>
+  <si>
+    <t>Olympus</t>
+  </si>
+  <si>
+    <t>EPL 1</t>
+  </si>
+  <si>
+    <t>EPL1 Camera</t>
+  </si>
+  <si>
+    <t>B3B505338</t>
+  </si>
+  <si>
+    <t>#Panny20mm</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Panasonic_Lumix_20mm_lens</t>
+  </si>
+  <si>
+    <t>Panasonic lens</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>Lumix G 20mm F1.7 Asph.</t>
+  </si>
+  <si>
+    <t>Lumix G 20/F1.7 lens</t>
+  </si>
+  <si>
+    <t>01FG3033651</t>
+  </si>
+  <si>
+    <t>agent</t>
+  </si>
+  <si>
+    <t>endTime</t>
+  </si>
+  <si>
+    <t>instrument</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>#Photo1</t>
+  </si>
+  <si>
+    <t>CreateAction</t>
+  </si>
+  <si>
+    <t>Photo snapped on a photo walk on a misty day</t>
+  </si>
+  <si>
+    <t>2017:06:11T12:56:14+10:00</t>
+  </si>
+  <si>
+    <t>["#EPL1", "#Panny20mm"]</t>
+  </si>
+  <si>
+    <t>Took dog picture</t>
+  </si>
+  <si>
+    <t>"pics/2017-06-11 12.56.14.jpg"</t>
+  </si>
+  <si>
+    <t>#SepiaConversion</t>
+  </si>
+  <si>
+    <t>convert -sepia-tone 80% test_data/sample/pics/2017-06-11\ 12.56.14.jpg test_data/sample/pics/sepia_fence.jpg</t>
+  </si>
+  <si>
+    <t>2018:09:19T17:01:07+10:00</t>
+  </si>
+  <si>
+    <t>"https://www.imagemagick.org/"</t>
+  </si>
+  <si>
+    <t>Converted dog picture to sepia</t>
+  </si>
+  <si>
+    <t>"pics/sepia_fence.jpg"</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>#picsdistro</t>
+  </si>
+  <si>
+    <t>DataDownload</t>
+  </si>
+  <si>
+    <t>http://data.research.uts.edu.au</t>
+  </si>
+  <si>
+    <t>https://data.research.uts.edu.au/examples/ro-crate/examples/src/downloads/sample.zip</t>
+  </si>
+  <si>
+    <t>[https://data.research.uts.edu.au/examples/ro-crate/examples/src/downloads/sample.zip, ]</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by-nc-sa/3.0/au/</t>
+  </si>
+  <si>
+    <t>CreativeWork</t>
+  </si>
+  <si>
+    <t>This work is licensed under the Creative Commons Attribution-NonCommercial-ShareAlike 3.0 Australia License. To view a copy of this license, visit http://creativecommons.org/licenses/by-nc-sa/3.0/au/ or send a letter to Creative Commons, PO Box 1866, Mountain View, CA 94042, USA.</t>
+  </si>
+  <si>
+    <t>Attribution-NonCommercial-ShareAlike 3.0 Australia (CC BY-NC-SA 3.0 AU)</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>https://www.imagemagick.org/</t>
+  </si>
+  <si>
+    <t>SoftwareApplication</t>
+  </si>
+  <si>
+    <t>ImageMagick</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ImageMagick 7.0.8-2 Q16 x86_64 2018-06-19</t>
+  </si>
+  <si>
+    <t>https://www.nationalarchives.gov.uk/PRONOM/fmt/645</t>
+  </si>
+  <si>
+    <t>website</t>
   </si>
   <si>
     <t>Exchangeable Image File Format (Compressed)</t>
   </si>
   <si>
-    <t>http://www.nationalarchives.gov.uk/PRONOM/fmt/645</t>
-  </si>
-  <si>
-    <t>"pics/thumbs/2017-06-11 12.56.14.png"</t>
-  </si>
-  <si>
-    <t>pics/sepia_fence.jpg</t>
-  </si>
-  <si>
-    <t>4855037</t>
-  </si>
-  <si>
-    <t>Sepia tone version of my fence/dog pic</t>
-  </si>
-  <si>
-    <t>JPEG File Interchange Format</t>
-  </si>
-  <si>
-    <t>http://www.nationalarchives.gov.uk/PRONOM/fmt/43</t>
-  </si>
-  <si>
-    <t>"pics/thumbs/sepia_fence.png"</t>
-  </si>
-  <si>
-    <t>pics/thumbs/2017-06-11 12.56.14.png</t>
-  </si>
-  <si>
-    <t>20594</t>
-  </si>
-  <si>
-    <t>Portable Network Graphics</t>
-  </si>
-  <si>
-    <t>http://www.nationalarchives.gov.uk/PRONOM/fmt/11</t>
-  </si>
-  <si>
-    <t>pics/thumbs/sepia_fence.png</t>
-  </si>
-  <si>
-    <t>20524</t>
-  </si>
-  <si>
-    <t>affiliation</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>familyName</t>
-  </si>
-  <si>
-    <t>givenName</t>
-  </si>
-  <si>
-    <t>http://orcid.org/0000-0002-3545-944X</t>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>mailto:peter.sefton@uts.edu.au</t>
-  </si>
-  <si>
-    <t>pt@ptsefton.com</t>
-  </si>
-  <si>
-    <t>Sefton</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Peter Sefton</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>http://ands.org.au</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>The core purpose of the Australian National Data Service (ANDS) is to make Australia’s research data assets more valuable for researchers, research institutions and the nation.</t>
-  </si>
-  <si>
-    <t>Australian National Data Service</t>
-  </si>
-  <si>
-    <t>http://eresearch.uts.edu.au/projects/provisioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The University of Technology Sydney Provisioner project is </t>
-  </si>
-  <si>
-    <t>Provisioner Project</t>
-  </si>
-  <si>
-    <t>["https://ror.org/0384j8v12", "http://ands.org.au"]</t>
-  </si>
-  <si>
-    <t>https://github.com/UTS-eResearch/projects/datacrate</t>
-  </si>
-  <si>
-    <t>The DataCrate project is to write the spec for DataCrate, of which this is an example. The DataCrate project is part of the University of Technology Sydney's Provisioner project, which was part-funded by the Australian National Data Service (ANDS) - now part of the Australian Research Data Commons (ARDC).</t>
-  </si>
-  <si>
-    <t>DataCrate Project</t>
-  </si>
-  <si>
-    <t>https://ror.org/0384j8v12</t>
-  </si>
-  <si>
-    <t>University of Technology Sydney</t>
-  </si>
-  <si>
-    <t>Broadway, 2007, NSW Australia</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>geo</t>
-  </si>
-  <si>
-    <t>http://www.geonames.org/8152662/catalina-park.html</t>
-  </si>
-  <si>
-    <t>Place</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Catalina_Park</t>
-  </si>
-  <si>
-    <t>Katoomba, NSW</t>
-  </si>
-  <si>
-    <t>Catalina Park is a disused motor racing venue, located at Katoomba, in the Blue Mountains, New South Wales, Australia, and is recognised as an Aboriginal Place due to the long association of the local Gundungarra and Darug clans to the area.</t>
-  </si>
-  <si>
-    <t>{"@id":"#3e53e101-db05-49ad-a988-d97e484c2310","@type":"GeoCoordinates","latitude":"-33.7152","longitude":"150.30119","name":"Latitude: -33.7152, Longitude: 150.30119"}</t>
-  </si>
-  <si>
-    <t>Catalina Park</t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.1000/123456</t>
-  </si>
-  <si>
-    <t>ScholarlyArticle</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>This is an example publication with a dodgy DOI</t>
-  </si>
-  <si>
-    <t>manufacturer</t>
-  </si>
-  <si>
-    <t>model</t>
-  </si>
-  <si>
-    <t>serialNumber</t>
-  </si>
-  <si>
-    <t>#EPL1</t>
-  </si>
-  <si>
-    <t>IndividualProduct</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Olympus_PEN_E-PL1</t>
-  </si>
-  <si>
-    <t>Olympus camera with Panasonic 20mm lens</t>
-  </si>
-  <si>
-    <t>Olympus</t>
-  </si>
-  <si>
-    <t>EPL 1</t>
-  </si>
-  <si>
-    <t>EPL1 Camera</t>
-  </si>
-  <si>
-    <t>B3B505338</t>
-  </si>
-  <si>
-    <t>#Panny20mm</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Panasonic_Lumix_20mm_lens</t>
-  </si>
-  <si>
-    <t>Panasonic lens</t>
-  </si>
-  <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
-    <t>Lumix G 20mm F1.7 Asph.</t>
-  </si>
-  <si>
-    <t>Lumix G 20/F1.7 lens</t>
-  </si>
-  <si>
-    <t>01FG3033651</t>
-  </si>
-  <si>
-    <t>agent</t>
-  </si>
-  <si>
-    <t>endTime</t>
-  </si>
-  <si>
-    <t>instrument</t>
-  </si>
-  <si>
-    <t>object</t>
-  </si>
-  <si>
-    <t>result</t>
-  </si>
-  <si>
-    <t>#Photo1</t>
-  </si>
-  <si>
-    <t>CreateAction</t>
-  </si>
-  <si>
-    <t>Photo snapped on a photo walk on a misty day</t>
-  </si>
-  <si>
-    <t>2017:06:11T12:56:14+10:00</t>
-  </si>
-  <si>
-    <t>["#EPL1", "#Panny20mm"]</t>
-  </si>
-  <si>
-    <t>Took dog picture</t>
-  </si>
-  <si>
-    <t>"pics/2017-06-11 12.56.14.jpg"</t>
-  </si>
-  <si>
-    <t>#SepiaConversion</t>
-  </si>
-  <si>
-    <t>convert -sepia-tone 80% test_data/sample/pics/2017-06-11\ 12.56.14.jpg test_data/sample/pics/sepia_fence.jpg</t>
-  </si>
-  <si>
-    <t>2018:09:19T17:01:07+10:00</t>
-  </si>
-  <si>
-    <t>"https://www.imagemagick.org/"</t>
-  </si>
-  <si>
-    <t>Converted dog picture to sepia</t>
-  </si>
-  <si>
-    <t>"pics/sepia_fence.jpg"</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>#picsdistro</t>
-  </si>
-  <si>
-    <t>DataDownload</t>
-  </si>
-  <si>
-    <t>http://data.research.uts.edu.au</t>
-  </si>
-  <si>
-    <t>https://data.research.uts.edu.au/examples/ro-crate/examples/src/downloads/sample.zip</t>
-  </si>
-  <si>
-    <t>[https://data.research.uts.edu.au/examples/ro-crate/examples/src/downloads/sample.zip, ]</t>
-  </si>
-  <si>
-    <t>zip</t>
-  </si>
-  <si>
-    <t>https://creativecommons.org/licenses/by-nc-sa/3.0/au/</t>
-  </si>
-  <si>
-    <t>CreativeWork</t>
-  </si>
-  <si>
-    <t>This work is licensed under the Creative Commons Attribution-NonCommercial-ShareAlike 3.0 Australia License. To view a copy of this license, visit http://creativecommons.org/licenses/by-nc-sa/3.0/au/ or send a letter to Creative Commons, PO Box 1866, Mountain View, CA 94042, USA.</t>
-  </si>
-  <si>
-    <t>Attribution-NonCommercial-ShareAlike 3.0 Australia (CC BY-NC-SA 3.0 AU)</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>https://www.imagemagick.org/</t>
-  </si>
-  <si>
-    <t>SoftwareApplication</t>
-  </si>
-  <si>
-    <t>ImageMagick</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ImageMagick 7.0.8-2 Q16 x86_64 2018-06-19</t>
-  </si>
-  <si>
     <t>https://www.nationalarchives.gov.uk/PRONOM/pronom</t>
-  </si>
-  <si>
-    <t>website</t>
   </si>
   <si>
     <t>Plain Text File</t>
@@ -1106,83 +1082,83 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="G1" t="s">
         <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="I1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="E2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="F2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="G2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F3" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="G3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="H3" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="I3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1207,44 +1183,44 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D1" t="s">
         <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1277,16 +1253,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1311,30 +1287,30 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
         <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1345,7 +1321,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
@@ -1364,13 +1340,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1395,10 +1382,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
         <v>28</v>
@@ -1406,19 +1393,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1469,13 +1456,13 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1488,39 +1475,42 @@
       <c r="D2" t="s">
         <v>36</v>
       </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1531,7 +1521,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="10" width="20" customWidth="1"/>
@@ -1545,246 +1535,150 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
         <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
         <v>28</v>
       </c>
       <c r="J1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2">
+        <v>5114778</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>50</v>
-      </c>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="C3">
+        <v>4855037</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4">
+        <v>20594</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
         <v>54</v>
       </c>
-      <c r="H3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>53</v>
-      </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="C5">
+        <v>20524</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I5" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" t="s">
         <v>68</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H7" t="s">
-        <v>76</v>
-      </c>
-      <c r="I7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1809,19 +1703,19 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H1" t="s">
         <v>28</v>
@@ -1829,28 +1723,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1884,52 +1778,52 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
         <v>31</v>
@@ -1937,22 +1831,22 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1977,16 +1871,16 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G1" t="s">
         <v>28</v>
@@ -1994,25 +1888,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2048,19 +1942,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2085,74 +1979,74 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="G1" t="s">
         <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="G2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" t="s">
         <v>122</v>
       </c>
-      <c r="C3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E3" t="s">
-        <v>132</v>
-      </c>
       <c r="F3" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="G3" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="H3" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed old, missing files
</commit_message>
<xml_diff>
--- a/sample-crate/ro-crate-metadata.xlsx
+++ b/sample-crate/ro-crate-metadata.xlsx
@@ -87,46 +87,46 @@
     <t>["http://ands.org.au", "https://ror.org/0384j8v12", "https://github.com/UTS-eResearch/projects/datacrate"]</t>
   </si>
   <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>https://dx.doi.org/10.5281/zenodo.1009240</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t>Dogs, Fences, The Gully</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>"https://creativecommons.org/licenses/by-nc-sa/3.0/au/"</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Sample dataset for RO-Crate v1.1</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>"https://ror.org/0384j8v12"</t>
+  </si>
+  <si>
+    <t>temporalCoverage</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
     <t>hasPart</t>
   </si>
   <si>
-    <t>["LICENSE", "README.md", "index.html", "lots_of_little_files/", "pics/"]</t>
-  </si>
-  <si>
-    <t>identifier</t>
-  </si>
-  <si>
-    <t>https://dx.doi.org/10.5281/zenodo.1009240</t>
-  </si>
-  <si>
-    <t>keywords</t>
-  </si>
-  <si>
-    <t>Dogs, Fences, The Gully</t>
-  </si>
-  <si>
-    <t>license</t>
-  </si>
-  <si>
-    <t>"https://creativecommons.org/licenses/by-nc-sa/3.0/au/"</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Sample dataset for RO-Crate v1.1</t>
-  </si>
-  <si>
-    <t>publisher</t>
-  </si>
-  <si>
-    <t>"https://ror.org/0384j8v12"</t>
-  </si>
-  <si>
-    <t>temporalCoverage</t>
-  </si>
-  <si>
-    <t>2017</t>
+    <t>["lots_of_little_files/", "pics/"]</t>
   </si>
   <si>
     <t>lots_of_little_files/</t>
@@ -1094,7 +1094,7 @@
         <v>128</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s">
         <v>129</v>
@@ -1186,7 +1186,7 @@
         <v>144</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
         <v>49</v>
@@ -1248,7 +1248,7 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1290,7 +1290,7 @@
         <v>95</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
         <v>155</v>
@@ -1335,7 +1335,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1388,7 +1388,7 @@
         <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1425,7 +1425,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1456,10 +1456,10 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1553,7 +1553,7 @@
         <v>50</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J1" t="s">
         <v>51</v>
@@ -1718,7 +1718,7 @@
         <v>72</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1729,7 +1729,7 @@
         <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>75</v>
@@ -1772,7 +1772,7 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
         <v>18</v>
@@ -1826,7 +1826,7 @@
         <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1883,7 +1883,7 @@
         <v>96</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1937,7 +1937,7 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1991,7 +1991,7 @@
         <v>109</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s">
         <v>110</v>

</xml_diff>